<commit_message>
updated experiment results and added new performance metrics files
</commit_message>
<xml_diff>
--- a/ours/phone/results/mean.xlsx
+++ b/ours/phone/results/mean.xlsx
@@ -948,7 +948,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Fine-tuned LLAMA-3.2-3B</t>
+          <t>LLAMA-3.2-3B (Fine-tuned)</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -979,7 +979,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Fine-tuned LLAMA-3.2-3B</t>
+          <t>LLAMA-3.2-3B (Fine-tuned)</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1010,7 +1010,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Fine-tuned LLAMA-3.2-3B</t>
+          <t>LLAMA-3.2-3B (Fine-tuned)</t>
         </is>
       </c>
       <c r="B19" t="n">

</xml_diff>